<commit_message>
guardar dataframe en un excel y csv
</commit_message>
<xml_diff>
--- a/datos_inmobiliarios.xlsx
+++ b/datos_inmobiliarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="163">
   <si>
     <t>Precio</t>
   </si>
@@ -43,24 +43,24 @@
     <t>San Pedro, Carabayllo, Perú</t>
   </si>
   <si>
+    <t>Playa Las Totoritas, Cañete, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Mala, Cañete</t>
+  </si>
+  <si>
+    <t>Avenida Metropolitana &amp; Avenida Prolongación Javier Prado Este, Ate, Perú</t>
+  </si>
+  <si>
+    <t>Santiago De Surco, Lima</t>
+  </si>
+  <si>
     <t>Bahia, Pueblo Libre, Perú</t>
   </si>
   <si>
     <t>San Borja, Lima</t>
   </si>
   <si>
-    <t>Playa Las Totoritas, Cañete, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Mala, Cañete</t>
-  </si>
-  <si>
-    <t>Avenida Metropolitana &amp; Avenida Prolongación Javier Prado Este, Ate, Perú</t>
-  </si>
-  <si>
-    <t>Santiago De Surco, Lima</t>
-  </si>
-  <si>
     <t>Rinconada Baja, Lima</t>
   </si>
   <si>
@@ -73,433 +73,436 @@
     <t>Punta Corrientes, Cerro Azul, Perú</t>
   </si>
   <si>
+    <t>Urb Portada De La Planicie, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Naplo, Pucusana, Perú</t>
+  </si>
+  <si>
+    <t>Calle Bahía 200-298, Cuadra 2, Co. La Molina Real, La Molina, Lima, 15026, Per</t>
+  </si>
+  <si>
+    <t>Lomas De La Molina Vieja, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Santa Cruz De Flores, Cañete, Lima, Per</t>
+  </si>
+  <si>
+    <t>El Sol De La Molina, Lima</t>
+  </si>
+  <si>
+    <t>Santa María, Huaura, Lima, Per</t>
+  </si>
+  <si>
+    <t>José María Quiroga 339, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>Cerros De Camacho, Santiago De Surco, Lima, Lima, Peru</t>
+  </si>
+  <si>
+    <t>Valle Hermoso, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>Calle Campo Verde 101-199, Cuadra 1, Ur. Campo Verde, La Molina, Lima, 15026, Per</t>
+  </si>
+  <si>
+    <t>Calle Las Dalias 338-368, Cuadra 3, Ur. Valle Hermoso Residencial Etapa Ii, Santiago De Surco, Lima, 15023, Per</t>
+  </si>
+  <si>
+    <t>Avenida San Borja Norte 1234, Lima, Perú</t>
+  </si>
+  <si>
+    <t>La Planicie, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Jirón El Mástil 515-577, Cuadra 5, Ur. Las Lagunas De La Molina Etapa Iii, La Molina, Lima, 15026, Per</t>
+  </si>
+  <si>
+    <t>Calle General Silva 685, Cuadra 6, Ur. San Antonio, Miraflores, Lima, 15047, Per</t>
+  </si>
+  <si>
+    <t>Jirón Coronel Enrique Campos, Surco, Perú</t>
+  </si>
+  <si>
+    <t>La Floristería, Jirón Simón Salguero, Ur. Residencial El Rosal, Santiago De Surco, Lima, 15048, Per</t>
+  </si>
+  <si>
     <t>Jirón Paseo De Los Eucaliptos 460, La Molina, Perú</t>
   </si>
   <si>
-    <t>Jirón Aragón 178, Pueblo Libre, Perú</t>
+    <t>Av. Rinconada Del Lago 915, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Viña Del Mar 131, Perú</t>
+  </si>
+  <si>
+    <t>Calle Pastor Sevilla, Chorrillos, Perú</t>
+  </si>
+  <si>
+    <t>Ricardo Angulo, San Isidro, Lima, Lima, Peru</t>
+  </si>
+  <si>
+    <t>Rinconada Alta, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Las Lagunas, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>La Planicie, 1a Etapa, 12, La Molina, Lima, Lima, Peru</t>
+  </si>
+  <si>
+    <t>Calle German Schreiber, Avenida Dos De Mayo, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Calle German Schreiber Gulsmanco 210, Calle German Schreiber Gulsmanco, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Pando, Lima</t>
+  </si>
+  <si>
+    <t>Jirón Cayaltí 241-279, Cuadra 2, Ur. Centro Comercial De Monterrico, Santiago De Surco, Lima, 15023, Per</t>
+  </si>
+  <si>
+    <t>Juan De La Fuente 905, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Urb Paso Chico, Paseo Paso Chico, Lurín, Perú</t>
+  </si>
+  <si>
+    <t>Pasaje Santa Rosa 865 Chaclacayo, Los Pinos, Los Halcones, Chaclacayo, Perú</t>
   </si>
   <si>
     <t>Daniel Urrea 251, Chorrillos, Lima 15063, Perú</t>
   </si>
   <si>
-    <t>La Planicie, La Molina, Perú</t>
+    <t>Carlos Monge Medrano, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>Cercado De Lima, Lima</t>
   </si>
   <si>
     <t>Calle Baltazar La Torre 3, San Isidro, Perú</t>
   </si>
   <si>
-    <t>Cerros De Camacho, Santiago De Surco, Lima, Lima, Peru</t>
-  </si>
-  <si>
-    <t>Calle Bahía 200-298, Cuadra 2, Co. La Molina Real, La Molina, Lima, 15026, Per</t>
-  </si>
-  <si>
-    <t>Lomas De La Molina Vieja, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Jirón Coronel Enrique Campos, Surco, Perú</t>
-  </si>
-  <si>
-    <t>Rinconada Alta, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Las Lagunas, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Santa Cruz De Flores, Cañete, Lima, Per</t>
-  </si>
-  <si>
-    <t>La Planicie, 1a Etapa, 12, La Molina, Lima, Lima, Peru</t>
-  </si>
-  <si>
-    <t>Calle Campo Verde 101-199, Cuadra 1, Ur. Campo Verde, La Molina, Lima, 15026, Per</t>
-  </si>
-  <si>
-    <t>José María Quiroga 339, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Calle Las Dalias 338-368, Cuadra 3, Ur. Valle Hermoso Residencial Etapa Ii, Santiago De Surco, Lima, 15023, Per</t>
-  </si>
-  <si>
-    <t>El Sol De La Molina, Lima</t>
-  </si>
-  <si>
-    <t>Jirón El Mástil 515-577, Cuadra 5, Ur. Las Lagunas De La Molina Etapa Iii, La Molina, Lima, 15026, Per</t>
-  </si>
-  <si>
-    <t>Valle Hermoso, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Urb Paso Chico, Paseo Paso Chico, Lurín, Perú</t>
-  </si>
-  <si>
-    <t>Ricardo Angulo, San Isidro, Lima, Lima, Peru</t>
-  </si>
-  <si>
-    <t>Avenida San Borja Norte 1234, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Calle Pastor Sevilla, Chorrillos, Perú</t>
+    <t>Mala, Cañete, Lima, Per</t>
+  </si>
+  <si>
+    <t>Calle Los Libertadores, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Jirón Eduardo Lizarzaburu, San Borja, Perú</t>
+  </si>
+  <si>
+    <t>Orrantia, Lima</t>
+  </si>
+  <si>
+    <t>Av. Andrés Aramburú, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Alameda Manuel Prado Ugarteche 400-478, Cuadra 4, Ot. Universidad Nacional Agraria, La Molina, Lima, 15024, Per</t>
+  </si>
+  <si>
+    <t>La Encantada 130, Rinconada Del Lago, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Rio De Janeiro 200, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Las Fresas, Lima 15048, Perú</t>
+  </si>
+  <si>
+    <t>Alberto Bartón, Santa Catalina, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Monte Álamo 255, Surco, Perú</t>
   </si>
   <si>
     <t>Avenida Las Casuarinas, Santiago De Surco, Perú</t>
   </si>
   <si>
-    <t>Calle General Silva 685, Cuadra 6, Ur. San Antonio, Miraflores, Lima, 15047, Per</t>
-  </si>
-  <si>
-    <t>Santa María, Huaura, Lima, Per</t>
-  </si>
-  <si>
-    <t>La Floristería, Jirón Simón Salguero, Ur. Residencial El Rosal, Santiago De Surco, Lima, 15048, Per</t>
+    <t>Avenida Paseo La Castellana 356, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>Calle Neiser Llacsa Arce, Lima, Perú</t>
   </si>
   <si>
     <t>Las Caobas, La Molina, Perú</t>
   </si>
   <si>
-    <t>Jirón Eduardo Lizarzaburu, San Borja, Perú</t>
-  </si>
-  <si>
-    <t>Camino Del Bosque, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Av. Rinconada Del Lago 915, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Monte Álamo 255, Surco, Perú</t>
+    <t>Pucusana, Perú</t>
   </si>
   <si>
     <t>Calle Castilla La Vieja, Surco, Perú</t>
   </si>
   <si>
-    <t>Viña Del Mar 131, Perú</t>
-  </si>
-  <si>
-    <t>Cercado De Lima, Lima</t>
-  </si>
-  <si>
-    <t>Maranga, San Miguel, Perú</t>
-  </si>
-  <si>
-    <t>Calle German Schreiber, Avenida Dos De Mayo, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Calle German Schreiber Gulsmanco 210, Calle German Schreiber Gulsmanco, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Jirón Cayaltí 241-279, Cuadra 2, Ur. Centro Comercial De Monterrico, Santiago De Surco, Lima, 15023, Per</t>
-  </si>
-  <si>
-    <t>Carlos Monge Medrano, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Juan De La Fuente 905, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Mala, Cañete, Lima, Per</t>
-  </si>
-  <si>
-    <t>Alameda Manuel Prado Ugarteche 400-478, Cuadra 4, Ot. Universidad Nacional Agraria, La Molina, Lima, 15024, Per</t>
-  </si>
-  <si>
-    <t>Rio De Janeiro 200, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Alberto Bartón, Santa Catalina, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Pando, Lima</t>
-  </si>
-  <si>
-    <t>La Encantada 130, Rinconada Del Lago, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Las Fresas, Lima 15048, Perú</t>
-  </si>
-  <si>
-    <t>La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Calle Neiser Llacsa Arce, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Naplo, Pucusana, Perú</t>
-  </si>
-  <si>
-    <t>Pasaje Santa Rosa 865 Chaclacayo, Los Pinos, Los Halcones, Chaclacayo, Perú</t>
-  </si>
-  <si>
-    <t>Orrantia, Lima</t>
-  </si>
-  <si>
-    <t>Avenida Paseo La Castellana 356, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Calle Los Libertadores, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Pucusana, Perú</t>
-  </si>
-  <si>
-    <t>Av. Andrés Aramburú, San Isidro, Perú</t>
+    <t>Urb California, Perú</t>
+  </si>
+  <si>
+    <t>Av. Pedro De Osma 417, Barranco, Perú</t>
+  </si>
+  <si>
+    <t>Chorrillos, Lima</t>
+  </si>
+  <si>
+    <t>El Haras 5, La Molina, Perú</t>
   </si>
   <si>
     <t>Calle Pulla De Raymondi, Lima, Perú</t>
   </si>
   <si>
-    <t>Urb California, Perú</t>
-  </si>
-  <si>
-    <t>El Haras 5, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Av. Pedro De Osma 417, Barranco, Perú</t>
-  </si>
-  <si>
-    <t>Chorrillos, Lima</t>
+    <t>Pachacamac, Lima</t>
   </si>
   <si>
     <t>Avenida Juan De Aliaga 400, Magdalena Del Mar, Perú</t>
   </si>
   <si>
-    <t>Pachacamac, Lima</t>
+    <t>Ivan Huerta, Cercado De Lima, Perú</t>
+  </si>
+  <si>
+    <t>Magdalena Del Mar, Lima</t>
+  </si>
+  <si>
+    <t>Surquillo, Lima</t>
   </si>
   <si>
     <t>Sevilla 115, Miraflores, Perú</t>
   </si>
   <si>
-    <t>Magdalena Del Mar, Lima</t>
-  </si>
-  <si>
-    <t>Ivan Huerta, Cercado De Lima, Perú</t>
-  </si>
-  <si>
-    <t>Surquillo, Lima</t>
+    <t>Jirón Madreselva, Surco, Perú</t>
+  </si>
+  <si>
+    <t>La Molina Vieja, La Molina, Perú</t>
   </si>
   <si>
     <t>Jirón Los Molles 267, Santiago De Surco, Perú</t>
   </si>
   <si>
-    <t>Jirón Madreselva, Surco, Perú</t>
-  </si>
-  <si>
     <t>Av. Belén, San Isidro, Perú</t>
   </si>
   <si>
+    <t>Punta Negra, Perú</t>
+  </si>
+  <si>
     <t>Cloegio Pamer, Avenida Los Alameda Horizontes 710, Cuadra 7, Ur. Los Cedros De Villa Etapa Iv, Chorrillos, Lima, 15067, Per</t>
   </si>
   <si>
-    <t>La Molina Vieja, La Molina, Perú</t>
-  </si>
-  <si>
     <t>Avenida Manuel Prado Ugarteche, La Molina, Perú</t>
   </si>
   <si>
+    <t>Surco, Perú</t>
+  </si>
+  <si>
+    <t>Jirón Maximiliano Carranza 856-898, Cuadra 8, Ur. San Juan Sector D, San Juan De Miraflores, Lima, 15801, Per</t>
+  </si>
+  <si>
     <t>Los Canarios, La Pradera, Lima, Perú</t>
   </si>
   <si>
-    <t>Jirón Maximiliano Carranza 856-898, Cuadra 8, Ur. San Juan Sector D, San Juan De Miraflores, Lima, 15801, Per</t>
-  </si>
-  <si>
-    <t>Surco, Perú</t>
+    <t>Capilla San Francisco De Asís, Avenida Buenos Aires, Chorrillos, Perú</t>
+  </si>
+  <si>
+    <t>San Martin De Porres, Lima</t>
   </si>
   <si>
     <t>Alameda El Triangulo, Urb Las Brisas De Villa, Lima, Perú</t>
   </si>
   <si>
+    <t>Jirón Batalla De Junin 300, Barranco, Perú</t>
+  </si>
+  <si>
+    <t>San Juan De Miraflores, Lima</t>
+  </si>
+  <si>
+    <t>Geronimo De Aliaga Norte, Surco, Perú</t>
+  </si>
+  <si>
+    <t>Ancon, Lima</t>
+  </si>
+  <si>
+    <t>Pueblo Libre, Lima</t>
+  </si>
+  <si>
+    <t>Calle Eduardo H. La Torre Villamonte 205, Urb El Rosal, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Calle Valle Riestra, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Aurelio Fernandez Concha, Miraflores, Perú</t>
+  </si>
+  <si>
+    <t>Cerezos 229, Micaela Bastidas, Los Olivos, Lima Province, Perú</t>
+  </si>
+  <si>
+    <t>Alameda Domingo Tristán Y Moscoso 520, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>El Paraiso, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>León De La Fuente, Magdalena Del Mar, Perú</t>
+  </si>
+  <si>
+    <t>Av. Ayacucho 1429, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>La Planicie, Lima</t>
+  </si>
+  <si>
+    <t>Avenida Manuel Olguín, Surco, Perú</t>
+  </si>
+  <si>
+    <t>Maranga, Lima</t>
+  </si>
+  <si>
+    <t>Calle Pedro Canga, San Isidro, Perú</t>
+  </si>
+  <si>
     <t>Calle Arias Araguez 601-699, Cuadra 6, Ur. San Antonio, Miraflores, Lima, 15047, Per</t>
   </si>
   <si>
-    <t>San Martin De Porres, Lima</t>
-  </si>
-  <si>
-    <t>San Juan De Miraflores, Lima</t>
-  </si>
-  <si>
-    <t>Pueblo Libre, Lima</t>
-  </si>
-  <si>
-    <t>Ancon, Lima</t>
-  </si>
-  <si>
-    <t>Alameda Domingo Tristán Y Moscoso 520, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Calle Valle Riestra, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Jirón Batalla De Junin 300, Barranco, Perú</t>
-  </si>
-  <si>
-    <t>Cerezos 229, Micaela Bastidas, Los Olivos, Lima Province, Perú</t>
-  </si>
-  <si>
-    <t>Geronimo De Aliaga Norte, Surco, Perú</t>
+    <t>Villa El Salvador, Lima</t>
+  </si>
+  <si>
+    <t>Los Sauces, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>Av. Gral. Francisco Valle Riestra 595, San Isidro 15076, Perú</t>
+  </si>
+  <si>
+    <t>Calle Los Pinos, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Jirón Bartolomé De Las Casas 400-488, Cuadra 4, Ur. Pablo Canepa, La Molina, Lima, 15012, Per</t>
+  </si>
+  <si>
+    <t>Club De Regatas "lima" · Filial La Cantuta, Circunvalacion, Lurigancho-chosica, Perú</t>
+  </si>
+  <si>
+    <t>Jirón Los Alamos 183, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Jirón Daniel Carrión 585, Magdalena Del Mar, Perú</t>
+  </si>
+  <si>
+    <t>Av. Pedro De Osma, Barranco, Perú</t>
+  </si>
+  <si>
+    <t>Calle General La Fuente 165, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Pasaje Los Lirios 192, Lurigancho-chosica, Perú</t>
+  </si>
+  <si>
+    <t>Playa La Encontrada, Asia, Perú</t>
+  </si>
+  <si>
+    <t>Las Higueras 200, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Las Palmas, Asia, Perú</t>
+  </si>
+  <si>
+    <t>Via Láctea 205, Santiago De Surco 15023, Perú</t>
+  </si>
+  <si>
+    <t>Batallon Tarma Surco, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Av. Bolívar, Cieneguilla, Perú</t>
+  </si>
+  <si>
+    <t>Jr. Hawai 1, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Tercera Etapa, Cieneguilla, Perú</t>
+  </si>
+  <si>
+    <t>Tambo Viejo, Cieneguilla, Perú</t>
+  </si>
+  <si>
+    <t>Calle Los Manzanos 315, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>El Olivar Desarrolladora, Raymundo Morales De La Torre, San Isidro, Lima, Peru</t>
+  </si>
+  <si>
+    <t>Av. Alejandro Iglesias 725, Chorrillos, Perú</t>
+  </si>
+  <si>
+    <t>Purus 170, Rímac, Perú</t>
+  </si>
+  <si>
+    <t>San Antonio, Lima</t>
+  </si>
+  <si>
+    <t>La Planicie, Lima, Perú</t>
+  </si>
+  <si>
+    <t>Jirón Juan De La Torre 200-222, Cuadra 2, Ur. Valle Hermoso Este, Santiago De Surco, Lima, 15023, Per</t>
   </si>
   <si>
     <t>Ricardo Palma, Urb Covima, La Molina, Perú</t>
   </si>
   <si>
-    <t>Aurelio Fernandez Concha, Miraflores, Perú</t>
-  </si>
-  <si>
-    <t>Maranga, Lima</t>
-  </si>
-  <si>
-    <t>Calle Pedro Canga, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Calle Eduardo H. La Torre Villamonte 205, Urb El Rosal, Lima, Perú</t>
-  </si>
-  <si>
-    <t>El Paraiso, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>León De La Fuente, Magdalena Del Mar, Perú</t>
-  </si>
-  <si>
-    <t>Avenida Manuel Olguín, Surco, Perú</t>
-  </si>
-  <si>
-    <t>Los Sauces, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Av. Ayacucho 1429, Santiago De Surco, Perú</t>
-  </si>
-  <si>
-    <t>Calle Los Pinos, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Jirón Los Alamos 183, Lima, Perú</t>
-  </si>
-  <si>
-    <t>La Planicie, Lima</t>
-  </si>
-  <si>
-    <t>Calle General La Fuente 165, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Av. Gral. Francisco Valle Riestra 595, San Isidro 15076, Perú</t>
-  </si>
-  <si>
-    <t>Villa El Salvador, Lima</t>
-  </si>
-  <si>
-    <t>Av. Pedro De Osma, Barranco, Perú</t>
-  </si>
-  <si>
-    <t>Jirón Daniel Carrión 585, Magdalena Del Mar, Perú</t>
-  </si>
-  <si>
-    <t>Jirón Bartolomé De Las Casas 400-488, Cuadra 4, Ur. Pablo Canepa, La Molina, Lima, 15012, Per</t>
-  </si>
-  <si>
-    <t>Club De Regatas "lima" · Filial La Cantuta, Circunvalacion, Lurigancho-chosica, Perú</t>
-  </si>
-  <si>
-    <t>Playa La Encontrada, Asia, Perú</t>
-  </si>
-  <si>
-    <t>Pasaje Los Lirios 192, Lurigancho-chosica, Perú</t>
-  </si>
-  <si>
-    <t>Avenida Virgen Del Carmen, Ur. Pro Etapa Vii, San Martín De Porres, Lima, 15113, Per</t>
-  </si>
-  <si>
-    <t>Av. Alejandro Iglesias 725, Chorrillos, Perú</t>
-  </si>
-  <si>
-    <t>Purus 170, Rímac, Perú</t>
-  </si>
-  <si>
-    <t>Via Láctea 205, Santiago De Surco 15023, Perú</t>
-  </si>
-  <si>
-    <t>Batallon Tarma Surco, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Tambo Viejo, Cieneguilla, Perú</t>
+    <t>Jirón Batallón Callao Norte, Cercado De Lima, Perú</t>
+  </si>
+  <si>
+    <t>Santa Cruz, Lima</t>
   </si>
   <si>
     <t>El Cascajal, Jirón El Cascajal, Surco, Perú</t>
   </si>
   <si>
-    <t>Jirón Juan De La Torre 200-222, Cuadra 2, Ur. Valle Hermoso Este, Santiago De Surco, Lima, 15023, Per</t>
-  </si>
-  <si>
-    <t>El Olivar Desarrolladora, Raymundo Morales De La Torre, San Isidro, Lima, Peru</t>
-  </si>
-  <si>
-    <t>La Planicie, Lima, Perú</t>
-  </si>
-  <si>
-    <t>Calle Los Manzanos 315, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Av. Bolívar, Cieneguilla, Perú</t>
-  </si>
-  <si>
-    <t>San Antonio, Lima</t>
-  </si>
-  <si>
-    <t>Jirón Batallón Callao Norte, Cercado De Lima, Perú</t>
-  </si>
-  <si>
-    <t>Santa Cruz, Lima</t>
-  </si>
-  <si>
     <t>Conde De La Vega Del Ren, Lima, Perú</t>
   </si>
   <si>
-    <t>Tercera Etapa, Cieneguilla, Perú</t>
-  </si>
-  <si>
     <t>El Horizonte 366, La Molina, Perú</t>
   </si>
   <si>
     <t>Avenida Los Frutales, La Molina, Perú</t>
   </si>
   <si>
-    <t>Playa Las Lomas, Cerro Azul, Perú</t>
-  </si>
-  <si>
     <t>Av. Manuel Villarán 184, Lima, Perú</t>
   </si>
   <si>
+    <t>Calle El Montículo 100-198, Cuadra 1, Ur. La Planicie, La Molina, Lima, 15026, Per</t>
+  </si>
+  <si>
+    <t>El Monticulo, La Molina, Perú</t>
+  </si>
+  <si>
+    <t>Ca. John Hassinger, Cercado De Lima, Perú</t>
+  </si>
+  <si>
+    <t>Calle Jose Granda, San Isidro, Perú</t>
+  </si>
+  <si>
     <t>Jirón Viña Lariena 200, Santiago De Surco, Perú</t>
   </si>
   <si>
-    <t>Calle El Montículo 100-198, Cuadra 1, Ur. La Planicie, La Molina, Lima, 15026, Per</t>
-  </si>
-  <si>
-    <t>El Monticulo, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>Ca. John Hassinger, Cercado De Lima, Perú</t>
-  </si>
-  <si>
-    <t>Calle Jose Granda, San Isidro, Perú</t>
-  </si>
-  <si>
-    <t>Las Palmas, Asia, Perú</t>
-  </si>
-  <si>
     <t>Urb Rinconada Alta Etapa 2, La Molina, Perú</t>
   </si>
   <si>
+    <t>Jiron Cerro San Francisco 522 Las Casuarinas Surco, Jirón Cerro San Francisco, Santiago De Surco, Perú</t>
+  </si>
+  <si>
+    <t>Residencial Praderas De Pariachi Iii Etapa, Calle 1, Ate, Perú</t>
+  </si>
+  <si>
+    <t>San Bartolo, Lima</t>
+  </si>
+  <si>
+    <t>Calle José Dionisio Anchorena, San Isidro, Perú</t>
+  </si>
+  <si>
+    <t>Calle Carlos Graña, San Isidro, Perú</t>
+  </si>
+  <si>
     <t>Calle Arica, Miraflores, Perú</t>
   </si>
   <si>
-    <t>Jr. Hawai 1, La Molina, Perú</t>
-  </si>
-  <si>
-    <t>C. Jr. Pumacahua Brigadier, Jesús María, Perú</t>
-  </si>
-  <si>
-    <t>Angélica Palma 184, San Miguel, Perú</t>
-  </si>
-  <si>
-    <t>La Chalana, La Molina, Perú</t>
+    <t>M2, San Juan De Lurigancho 15427, Perú</t>
   </si>
 </sst>
 </file>
@@ -899,7 +902,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>5255733</v>
+        <v>5271826</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -916,7 +919,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>4447159</v>
+        <v>4460776</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -933,7 +936,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>5120971</v>
+        <v>5136651</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -949,99 +952,99 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6">
-        <v>550000</v>
-      </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>295</v>
+        <v>250</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7">
-        <v>850000</v>
-      </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>429</v>
+        <v>200</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8">
+        <v>340000</v>
+      </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
+      <c r="A9">
+        <v>699000</v>
+      </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>340000</v>
+        <v>550000</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10">
-        <v>156</v>
+        <v>295</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>699000</v>
+        <v>850000</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>400</v>
+        <v>429</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1080,36 +1083,36 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>387188</v>
+        <v>750000</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>178</v>
+        <v>700</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>750000</v>
+        <v>387188</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>700</v>
+        <v>178</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1165,101 +1168,101 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>1353450</v>
+        <v>850000</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>618</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>390000</v>
+        <v>700000</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
-        <v>223</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>490000</v>
+        <v>405000</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>240</v>
+        <v>178</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>1250000</v>
+        <v>570000</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>1000000</v>
+        <v>399000</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23">
-        <v>365</v>
+        <v>280</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>1220000</v>
+        <v>1047000</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -1267,101 +1270,101 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>940000</v>
+        <v>253000</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>563</v>
+        <v>679</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>570000</v>
+        <v>595000</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>399000</v>
+        <v>97000</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27">
-        <v>280</v>
+        <v>136</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>405000</v>
+        <v>615000</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C28">
-        <v>178</v>
+        <v>316</v>
       </c>
       <c r="D28">
         <v>4</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>680000</v>
+        <v>940000</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="C29">
-        <v>300</v>
+        <v>563</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>1047000</v>
+        <v>799000</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>595</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -1369,33 +1372,33 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>2100000</v>
+        <v>410000</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>202</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>980000</v>
+        <v>720000</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>461</v>
+        <v>600</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -1403,98 +1406,98 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>253000</v>
+        <v>800000</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33">
-        <v>679</v>
+        <v>480</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>3600000</v>
+        <v>253900</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>679</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>410000</v>
+        <v>1250000</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
       </c>
       <c r="C35">
-        <v>202</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>615000</v>
+        <v>600000</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
       </c>
       <c r="C36">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <v>2100000</v>
+        <v>850000</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <v>720000</v>
+        <v>680000</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C38">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1505,121 +1508,121 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
-        <v>1700000</v>
+        <v>399500</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
-        <v>595000</v>
+        <v>1220000</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <v>600000</v>
+        <v>1353450</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C41">
-        <v>290</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>5</v>
       </c>
       <c r="E41">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <v>799000</v>
+        <v>1400000</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C42">
-        <v>595</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
-        <v>1200000</v>
+        <v>475000</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>398</v>
       </c>
       <c r="D43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44">
-        <v>2100000</v>
+        <v>540000</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>592</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45">
-        <v>425000</v>
+        <v>389000</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>281</v>
       </c>
       <c r="D45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E45">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1627,7 +1630,7 @@
         <v>625000</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>360</v>
@@ -1641,220 +1644,220 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47">
-        <v>800000</v>
+        <v>2100000</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C47">
-        <v>480</v>
+        <v>2</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48">
-        <v>389000</v>
+        <v>980000</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C48">
-        <v>281</v>
+        <v>461</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49">
-        <v>579800</v>
+        <v>3600000</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C49">
-        <v>342</v>
+        <v>3</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50">
-        <v>253900</v>
+        <v>420000</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C50">
-        <v>679</v>
+        <v>269</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51">
-        <v>850000</v>
+        <v>2100000</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51">
-        <v>481</v>
+        <v>2</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E51">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52">
-        <v>97000</v>
+        <v>1700000</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C52">
-        <v>136</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53">
-        <v>399500</v>
+        <v>260000</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C53">
-        <v>202</v>
+        <v>140</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54">
-        <v>630000</v>
+        <v>1200000</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>332</v>
+        <v>1</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E54">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55">
-        <v>439000</v>
+        <v>2100000</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C55">
-        <v>212</v>
+        <v>2</v>
       </c>
       <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
         <v>6</v>
-      </c>
-      <c r="E55">
-        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56">
-        <v>399000</v>
+        <v>330000</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E56">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57">
-        <v>475000</v>
+        <v>549000</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C57">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58">
-        <v>370000</v>
+        <v>520000</v>
       </c>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C58">
-        <v>200</v>
+        <v>303</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59">
-        <v>415000</v>
+        <v>435000</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C59">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E59">
         <v>3</v>
@@ -1862,67 +1865,67 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60">
-        <v>1400000</v>
+        <v>425000</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61">
-        <v>540000</v>
+        <v>350000</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C61">
-        <v>592</v>
+        <v>300</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62">
-        <v>590000</v>
+        <v>490000</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C62">
-        <v>380</v>
+        <v>240</v>
       </c>
       <c r="D62">
         <v>4</v>
       </c>
       <c r="E62">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63">
-        <v>645000</v>
+        <v>560000</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="D63">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -1930,104 +1933,104 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64">
-        <v>420000</v>
+        <v>590000</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64">
-        <v>269</v>
+        <v>380</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65">
-        <v>260000</v>
+        <v>1000000</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C65">
-        <v>140</v>
+        <v>365</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66">
-        <v>549000</v>
+        <v>1260000</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C66">
-        <v>409</v>
+        <v>70</v>
       </c>
       <c r="D66">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67">
-        <v>560000</v>
+        <v>930000</v>
       </c>
       <c r="B67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C67">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="D67">
         <v>3</v>
       </c>
       <c r="E67">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68">
-        <v>520000</v>
+        <v>439000</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C68">
-        <v>303</v>
+        <v>212</v>
       </c>
       <c r="D68">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69">
-        <v>1260000</v>
+        <v>1270000</v>
       </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C69">
-        <v>70</v>
+        <v>345</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2035,98 +2038,98 @@
         <v>750000</v>
       </c>
       <c r="B70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C70">
-        <v>492</v>
+        <v>360</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E70">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71">
-        <v>695000</v>
+        <v>750000</v>
       </c>
       <c r="B71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C71">
-        <v>340</v>
+        <v>492</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E71">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72">
-        <v>325000</v>
+        <v>360000</v>
       </c>
       <c r="B72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C72">
-        <v>160</v>
+        <v>253</v>
       </c>
       <c r="D72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73">
-        <v>330000</v>
+        <v>695000</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73">
-        <v>240</v>
+        <v>340</v>
       </c>
       <c r="D73">
         <v>3</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74">
-        <v>360000</v>
+        <v>675000</v>
       </c>
       <c r="B74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C74">
-        <v>253</v>
+        <v>360</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E74">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75">
-        <v>435000</v>
+        <v>325000</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C75">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="D75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E75">
         <v>3</v>
@@ -2134,47 +2137,47 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76">
-        <v>675000</v>
+        <v>370000</v>
       </c>
       <c r="B76" t="s">
         <v>66</v>
       </c>
       <c r="C76">
-        <v>360</v>
+        <v>200</v>
       </c>
       <c r="D76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E76">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77">
-        <v>850000</v>
+        <v>1050000</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C77">
-        <v>618</v>
+        <v>378</v>
       </c>
       <c r="D77">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E77">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78">
-        <v>580000</v>
+        <v>579800</v>
       </c>
       <c r="B78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C78">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -2185,84 +2188,84 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79">
-        <v>700000</v>
+        <v>590000</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>327</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80">
-        <v>350000</v>
+        <v>580000</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80">
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E80">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81">
-        <v>1270000</v>
+        <v>630000</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C81">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82">
-        <v>590000</v>
+        <v>950000</v>
       </c>
       <c r="B82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C82">
-        <v>327</v>
+        <v>30</v>
       </c>
       <c r="D82">
         <v>4</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83">
-        <v>930000</v>
+        <v>415000</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C83">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E83">
         <v>3</v>
@@ -2270,67 +2273,67 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84">
-        <v>950000</v>
+        <v>500000</v>
       </c>
       <c r="B84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C84">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D84">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E84">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85">
-        <v>1050000</v>
+        <v>2500000</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C85">
-        <v>378</v>
+        <v>847</v>
       </c>
       <c r="D85">
         <v>3</v>
       </c>
       <c r="E85">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86">
-        <v>750000</v>
+        <v>475000</v>
       </c>
       <c r="B86" t="s">
         <v>75</v>
       </c>
       <c r="C86">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="D86">
         <v>4</v>
       </c>
       <c r="E86">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87">
-        <v>465000</v>
+        <v>890000</v>
       </c>
       <c r="B87" t="s">
         <v>76</v>
       </c>
       <c r="C87">
-        <v>312</v>
+        <v>600</v>
       </c>
       <c r="D87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E87">
         <v>3</v>
@@ -2338,75 +2341,75 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88">
-        <v>500000</v>
+        <v>465000</v>
       </c>
       <c r="B88" t="s">
         <v>77</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>312</v>
       </c>
       <c r="D88">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E88">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89">
-        <v>890000</v>
+        <v>1820000</v>
       </c>
       <c r="B89" t="s">
         <v>78</v>
       </c>
       <c r="C89">
-        <v>600</v>
+        <v>4</v>
       </c>
       <c r="D89">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E89">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90">
-        <v>2500000</v>
+        <v>1480000</v>
       </c>
       <c r="B90" t="s">
         <v>79</v>
       </c>
       <c r="C90">
-        <v>847</v>
+        <v>423</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E90">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91">
-        <v>475000</v>
+        <v>540000</v>
       </c>
       <c r="B91" t="s">
         <v>80</v>
       </c>
       <c r="C91">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92">
-        <v>1480000</v>
+        <v>320000</v>
       </c>
       <c r="B92" t="s">
         <v>81</v>
       </c>
       <c r="C92">
-        <v>423</v>
+        <v>70</v>
       </c>
       <c r="D92">
         <v>3</v>
@@ -2417,87 +2420,87 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93">
-        <v>1820000</v>
+        <v>470000</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C93">
-        <v>4</v>
+        <v>292</v>
       </c>
       <c r="D93">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E93">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94">
-        <v>825000</v>
+        <v>190000</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C94">
-        <v>267</v>
+        <v>110</v>
       </c>
       <c r="D94">
         <v>3</v>
       </c>
       <c r="E94">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95">
-        <v>320000</v>
+        <v>825000</v>
       </c>
       <c r="B95" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C95">
-        <v>70</v>
+        <v>267</v>
       </c>
       <c r="D95">
         <v>3</v>
       </c>
       <c r="E95">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96">
-        <v>540000</v>
+        <v>690000</v>
       </c>
       <c r="B96" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C96">
-        <v>200</v>
+        <v>415</v>
       </c>
       <c r="D96">
         <v>4</v>
       </c>
       <c r="E96">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97">
-        <v>190000</v>
+        <v>1200000</v>
       </c>
       <c r="B97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C97">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2505,7 +2508,7 @@
         <v>2000000</v>
       </c>
       <c r="B98" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -2519,16 +2522,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99">
-        <v>690000</v>
+        <v>1290000</v>
       </c>
       <c r="B99" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C99">
-        <v>415</v>
+        <v>498</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E99">
         <v>4</v>
@@ -2536,19 +2539,19 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100">
-        <v>1290000</v>
+        <v>220000</v>
       </c>
       <c r="B100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C100">
-        <v>498</v>
+        <v>264</v>
       </c>
       <c r="D100">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E100">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2556,7 +2559,7 @@
         <v>618000</v>
       </c>
       <c r="B101" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -2570,87 +2573,87 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102">
-        <v>470000</v>
+        <v>215000</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="C102">
-        <v>292</v>
+        <v>236</v>
       </c>
       <c r="D102">
         <v>5</v>
       </c>
       <c r="E102">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103">
-        <v>215000</v>
+        <v>399000</v>
       </c>
       <c r="B103" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>236</v>
+        <v>160</v>
       </c>
       <c r="D103">
         <v>5</v>
       </c>
       <c r="E103">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104">
-        <v>1200000</v>
+        <v>915000</v>
       </c>
       <c r="B104" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="D104">
         <v>4</v>
       </c>
       <c r="E104">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105">
-        <v>399000</v>
+        <v>500000</v>
       </c>
       <c r="B105" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="C105">
-        <v>160</v>
+        <v>500</v>
       </c>
       <c r="D105">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E105">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106">
-        <v>915000</v>
+        <v>230000</v>
       </c>
       <c r="B106" t="s">
         <v>92</v>
       </c>
       <c r="C106">
-        <v>540</v>
+        <v>225</v>
       </c>
       <c r="D106">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E106">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2672,36 +2675,36 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108">
-        <v>230000</v>
+        <v>179000</v>
       </c>
       <c r="B108" t="s">
         <v>94</v>
       </c>
       <c r="C108">
-        <v>225</v>
+        <v>100</v>
       </c>
       <c r="D108">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E108">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109">
-        <v>500000</v>
+        <v>240000</v>
       </c>
       <c r="B109" t="s">
         <v>95</v>
       </c>
       <c r="C109">
-        <v>500</v>
+        <v>111</v>
       </c>
       <c r="D109">
         <v>4</v>
       </c>
       <c r="E109">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2715,72 +2718,72 @@
         <v>600</v>
       </c>
       <c r="D110">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E110">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111">
-        <v>600000</v>
+        <v>2900000</v>
       </c>
       <c r="B111" t="s">
         <v>97</v>
       </c>
       <c r="C111">
-        <v>368</v>
+        <v>951</v>
       </c>
       <c r="D111">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E111">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112">
-        <v>240000</v>
+        <v>188000</v>
       </c>
       <c r="B112" t="s">
         <v>98</v>
       </c>
       <c r="C112">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="D112">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E112">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113">
-        <v>188000</v>
+        <v>720000</v>
       </c>
       <c r="B113" t="s">
         <v>99</v>
       </c>
       <c r="C113">
-        <v>160</v>
+        <v>362</v>
       </c>
       <c r="D113">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E113">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114">
-        <v>354000</v>
+        <v>795000</v>
       </c>
       <c r="B114" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="C114">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="D114">
         <v>2</v>
@@ -2794,30 +2797,30 @@
         <v>55000</v>
       </c>
       <c r="B115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C115">
         <v>160</v>
       </c>
       <c r="D115">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E115">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116">
-        <v>795000</v>
+        <v>354000</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="C116">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D116">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E116">
         <v>4</v>
@@ -2825,13 +2828,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117">
-        <v>286900</v>
+        <v>650000</v>
       </c>
       <c r="B117" t="s">
         <v>102</v>
       </c>
       <c r="C117">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="D117">
         <v>7</v>
@@ -2851,21 +2854,21 @@
         <v>507</v>
       </c>
       <c r="D118">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E118">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119">
-        <v>2900000</v>
+        <v>890000</v>
       </c>
       <c r="B119" t="s">
         <v>104</v>
       </c>
       <c r="C119">
-        <v>951</v>
+        <v>497</v>
       </c>
       <c r="D119">
         <v>12</v>
@@ -2885,120 +2888,120 @@
         <v>160</v>
       </c>
       <c r="D120">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E120">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121">
-        <v>720000</v>
+        <v>286900</v>
       </c>
       <c r="B121" t="s">
         <v>106</v>
       </c>
       <c r="C121">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122">
-        <v>315000</v>
+        <v>640000</v>
       </c>
       <c r="B122" t="s">
         <v>107</v>
       </c>
       <c r="C122">
-        <v>352</v>
+        <v>512</v>
       </c>
       <c r="D122">
         <v>3</v>
       </c>
       <c r="E122">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123">
-        <v>890000</v>
+        <v>650000</v>
       </c>
       <c r="B123" t="s">
         <v>108</v>
       </c>
       <c r="C123">
-        <v>497</v>
+        <v>305</v>
       </c>
       <c r="D123">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E123">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124">
-        <v>370000</v>
+        <v>495000</v>
       </c>
       <c r="B124" t="s">
         <v>109</v>
       </c>
       <c r="C124">
-        <v>160</v>
+        <v>300</v>
       </c>
       <c r="D124">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E124">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125">
-        <v>1700000</v>
+        <v>675000</v>
       </c>
       <c r="B125" t="s">
         <v>110</v>
       </c>
       <c r="C125">
-        <v>550</v>
+        <v>298</v>
       </c>
       <c r="D125">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E125">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126">
-        <v>650000</v>
+        <v>396000</v>
       </c>
       <c r="B126" t="s">
         <v>111</v>
       </c>
       <c r="C126">
-        <v>344</v>
+        <v>220</v>
       </c>
       <c r="D126">
         <v>4</v>
       </c>
       <c r="E126">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127">
-        <v>640000</v>
+        <v>370000</v>
       </c>
       <c r="B127" t="s">
         <v>112</v>
       </c>
       <c r="C127">
-        <v>512</v>
+        <v>160</v>
       </c>
       <c r="D127">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E127">
         <v>3</v>
@@ -3006,67 +3009,67 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128">
-        <v>650000</v>
+        <v>198000</v>
       </c>
       <c r="B128" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C128">
-        <v>305</v>
+        <v>240</v>
       </c>
       <c r="D128">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E128">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129">
-        <v>396000</v>
+        <v>1700000</v>
       </c>
       <c r="B129" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C129">
-        <v>220</v>
+        <v>550</v>
       </c>
       <c r="D129">
         <v>4</v>
       </c>
       <c r="E129">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130">
-        <v>2000000</v>
+        <v>600000</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C130">
-        <v>1</v>
+        <v>368</v>
       </c>
       <c r="D130">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E130">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131">
-        <v>495000</v>
+        <v>168500</v>
       </c>
       <c r="B131" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C131">
-        <v>300</v>
+        <v>335</v>
       </c>
       <c r="D131">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -3074,98 +3077,98 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132">
-        <v>1950000</v>
+        <v>800000</v>
       </c>
       <c r="B132" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C132">
-        <v>400</v>
+        <v>461</v>
       </c>
       <c r="D132">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E132">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133">
-        <v>898000</v>
+        <v>2000000</v>
       </c>
       <c r="B133" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C133">
-        <v>376</v>
+        <v>1</v>
       </c>
       <c r="D133">
         <v>4</v>
       </c>
       <c r="E133">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134">
-        <v>675000</v>
+        <v>1290000</v>
       </c>
       <c r="B134" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C134">
-        <v>298</v>
+        <v>507</v>
       </c>
       <c r="D134">
         <v>5</v>
       </c>
       <c r="E134">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135">
-        <v>998000</v>
+        <v>1950000</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C135">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="D135">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E135">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136">
-        <v>1290000</v>
+        <v>499000</v>
       </c>
       <c r="B136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C136">
-        <v>507</v>
+        <v>219</v>
       </c>
       <c r="D136">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E136">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137">
-        <v>198000</v>
+        <v>449500</v>
       </c>
       <c r="B137" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C137">
-        <v>240</v>
+        <v>1</v>
       </c>
       <c r="D137">
         <v>4</v>
@@ -3176,16 +3179,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138">
-        <v>168500</v>
+        <v>898000</v>
       </c>
       <c r="B138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C138">
-        <v>335</v>
+        <v>376</v>
       </c>
       <c r="D138">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E138">
         <v>4</v>
@@ -3193,13 +3196,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139">
-        <v>620000</v>
+        <v>600000</v>
       </c>
       <c r="B139" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C139">
-        <v>247</v>
+        <v>359</v>
       </c>
       <c r="D139">
         <v>3</v>
@@ -3210,13 +3213,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140">
-        <v>600000</v>
+        <v>620000</v>
       </c>
       <c r="B140" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C140">
-        <v>359</v>
+        <v>247</v>
       </c>
       <c r="D140">
         <v>3</v>
@@ -3227,84 +3230,84 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141">
-        <v>600000</v>
+        <v>998000</v>
       </c>
       <c r="B141" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="C141">
-        <v>240</v>
+        <v>391</v>
       </c>
       <c r="D141">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E141">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142">
-        <v>499000</v>
+        <v>265000</v>
       </c>
       <c r="B142" t="s">
         <v>125</v>
       </c>
       <c r="C142">
-        <v>219</v>
+        <v>504</v>
       </c>
       <c r="D142">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E142">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143">
-        <v>449500</v>
+        <v>123000</v>
       </c>
       <c r="B143" t="s">
         <v>126</v>
       </c>
       <c r="C143">
+        <v>100</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143">
         <v>1</v>
-      </c>
-      <c r="D143">
-        <v>4</v>
-      </c>
-      <c r="E143">
-        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144">
-        <v>123000</v>
+        <v>600000</v>
       </c>
       <c r="B144" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="C144">
-        <v>100</v>
+        <v>240</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145">
-        <v>265000</v>
+        <v>1050000</v>
       </c>
       <c r="B145" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C145">
-        <v>504</v>
+        <v>1</v>
       </c>
       <c r="D145">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E145">
         <v>3</v>
@@ -3312,16 +3315,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146">
-        <v>195000</v>
+        <v>350000</v>
       </c>
       <c r="B146" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C146">
-        <v>230</v>
+        <v>140</v>
       </c>
       <c r="D146">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E146">
         <v>3</v>
@@ -3329,13 +3332,13 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147">
-        <v>178000</v>
+        <v>730000</v>
       </c>
       <c r="B147" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C147">
-        <v>160</v>
+        <v>425</v>
       </c>
       <c r="D147">
         <v>5</v>
@@ -3345,11 +3348,14 @@
       </c>
     </row>
     <row r="148" spans="1:5">
+      <c r="A148">
+        <v>560000</v>
+      </c>
       <c r="B148" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C148">
-        <v>800</v>
+        <v>168</v>
       </c>
       <c r="D148">
         <v>3</v>
@@ -3360,13 +3366,13 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149">
-        <v>730000</v>
+        <v>135000</v>
       </c>
       <c r="B149" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C149">
-        <v>425</v>
+        <v>300</v>
       </c>
       <c r="D149">
         <v>4</v>
@@ -3377,32 +3383,44 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150">
-        <v>560000</v>
+        <v>417000</v>
       </c>
       <c r="B150" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C150">
-        <v>168</v>
+        <v>300</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+      <c r="E150">
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151">
-        <v>475000</v>
+        <v>180</v>
       </c>
       <c r="B151" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>230</v>
+      </c>
+      <c r="D151">
+        <v>3</v>
+      </c>
+      <c r="E151">
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152">
-        <v>3800000</v>
+        <v>475000</v>
       </c>
       <c r="B152" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3411,69 +3429,66 @@
         <v>4</v>
       </c>
       <c r="E152">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153">
-        <v>560000</v>
+        <v>1150000</v>
       </c>
       <c r="B153" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C153">
-        <v>310</v>
+        <v>602</v>
       </c>
       <c r="D153">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E153">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154">
-        <v>580000</v>
+        <v>2300000</v>
       </c>
       <c r="B154" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C154">
-        <v>2</v>
+        <v>505</v>
       </c>
       <c r="D154">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E154">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155">
-        <v>2300000</v>
+        <v>178000</v>
       </c>
       <c r="B155" t="s">
         <v>137</v>
       </c>
       <c r="C155">
-        <v>505</v>
+        <v>160</v>
       </c>
       <c r="D155">
         <v>4</v>
       </c>
       <c r="E155">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156">
-        <v>1350000</v>
-      </c>
       <c r="B156" t="s">
         <v>138</v>
       </c>
       <c r="C156">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="D156">
         <v>4</v>
@@ -3484,50 +3499,50 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157">
-        <v>1150000</v>
+        <v>650000</v>
       </c>
       <c r="B157" t="s">
         <v>139</v>
       </c>
       <c r="C157">
-        <v>602</v>
+        <v>1</v>
       </c>
       <c r="D157">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E157">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158">
-        <v>135000</v>
+        <v>1350000</v>
       </c>
       <c r="B158" t="s">
         <v>140</v>
       </c>
       <c r="C158">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="D158">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E158">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159">
-        <v>800000</v>
+        <v>560000</v>
       </c>
       <c r="B159" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="C159">
-        <v>461</v>
+        <v>352</v>
       </c>
       <c r="D159">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E159">
         <v>4</v>
@@ -3535,10 +3550,10 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160">
-        <v>650000</v>
+        <v>315000</v>
       </c>
       <c r="B160" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C160">
         <v>628</v>
@@ -3547,7 +3562,7 @@
         <v>4</v>
       </c>
       <c r="E160">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3555,16 +3570,16 @@
         <v>900000</v>
       </c>
       <c r="B161" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C161">
         <v>367</v>
       </c>
       <c r="D161">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E161">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3572,30 +3587,30 @@
         <v>750000</v>
       </c>
       <c r="B162" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C162">
-        <v>383</v>
+        <v>1</v>
       </c>
       <c r="D162">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E162">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163">
-        <v>670000</v>
+        <v>3800000</v>
       </c>
       <c r="B163" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C163">
-        <v>230</v>
+        <v>383</v>
       </c>
       <c r="D163">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E163">
         <v>4</v>
@@ -3603,10 +3618,10 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164">
-        <v>180</v>
+        <v>670000</v>
       </c>
       <c r="B164" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -3615,7 +3630,7 @@
         <v>3</v>
       </c>
       <c r="E164">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3623,16 +3638,16 @@
         <v>1697000</v>
       </c>
       <c r="B165" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C165">
         <v>318</v>
       </c>
       <c r="D165">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E165">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3640,10 +3655,10 @@
         <v>950000</v>
       </c>
       <c r="B166" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C166">
-        <v>410</v>
+        <v>630</v>
       </c>
       <c r="D166">
         <v>3</v>
@@ -3654,47 +3669,47 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167">
-        <v>449000</v>
+        <v>1180000</v>
       </c>
       <c r="B167" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C167">
-        <v>630</v>
+        <v>700</v>
       </c>
       <c r="D167">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E167">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:5">
       <c r="A168">
-        <v>1180000</v>
+        <v>900000</v>
       </c>
       <c r="B168" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C168">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="D168">
         <v>6</v>
       </c>
       <c r="E168">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:5">
       <c r="A169">
-        <v>300000</v>
+        <v>1190000</v>
       </c>
       <c r="B169" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C169">
-        <v>700</v>
+        <v>540</v>
       </c>
       <c r="D169">
         <v>4</v>
@@ -3705,132 +3720,132 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170">
-        <v>900000</v>
+        <v>650000</v>
       </c>
       <c r="B170" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C170">
-        <v>306</v>
+        <v>183</v>
       </c>
       <c r="D170">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E170">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="171" spans="1:5">
       <c r="A171">
-        <v>1190000</v>
+        <v>1389000</v>
       </c>
       <c r="B171" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C171">
-        <v>153</v>
+        <v>1</v>
       </c>
       <c r="D171">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E171">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:5">
       <c r="A172">
-        <v>524000</v>
+        <v>300000</v>
       </c>
       <c r="B172" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="C172">
-        <v>540</v>
+        <v>1</v>
       </c>
       <c r="D172">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E172">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:5">
       <c r="A173">
-        <v>650000</v>
+        <v>890000</v>
       </c>
       <c r="B173" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C173">
-        <v>140</v>
+        <v>244</v>
       </c>
       <c r="D173">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E173">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174" spans="1:5">
       <c r="A174">
-        <v>1389000</v>
+        <v>3112840</v>
       </c>
       <c r="B174" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C174">
         <v>1</v>
       </c>
       <c r="D174">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E174">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:5">
       <c r="A175">
-        <v>350000</v>
+        <v>320000</v>
       </c>
       <c r="B175" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C175">
-        <v>600</v>
+        <v>347</v>
       </c>
       <c r="D175">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E175">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176">
-        <v>890000</v>
+        <v>850000</v>
       </c>
       <c r="B176" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C176">
-        <v>300</v>
+        <v>723</v>
       </c>
       <c r="D176">
         <v>4</v>
       </c>
       <c r="E176">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:5">
       <c r="A177">
-        <v>1850000</v>
+        <v>1090000</v>
       </c>
       <c r="B177" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C177">
-        <v>240</v>
+        <v>600</v>
       </c>
       <c r="D177">
         <v>4</v>
@@ -3841,70 +3856,58 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178">
-        <v>417000</v>
+        <v>3800000</v>
       </c>
       <c r="B178" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C178">
-        <v>261</v>
+        <v>306</v>
       </c>
       <c r="D178">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E178">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:5">
       <c r="A179">
-        <v>270000</v>
+        <v>1850000</v>
       </c>
       <c r="B179" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C179">
-        <v>310</v>
+        <v>463</v>
       </c>
       <c r="D179">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E179">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:5">
       <c r="A180">
-        <v>330000</v>
+        <v>524000</v>
       </c>
       <c r="B180" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="C180">
         <v>0</v>
       </c>
-      <c r="D180">
-        <v>6</v>
-      </c>
-      <c r="E180">
-        <v>4</v>
-      </c>
     </row>
     <row r="181" spans="1:5">
       <c r="A181">
-        <v>490000</v>
+        <v>314000</v>
       </c>
       <c r="B181" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C181">
         <v>0</v>
-      </c>
-      <c r="D181">
-        <v>3</v>
-      </c>
-      <c r="E181">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>